<commit_message>
script can upload update units, but not clean code
</commit_message>
<xml_diff>
--- a/input/cdm-country-code.xlsx
+++ b/input/cdm-country-code.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickchandra/Documents/code/CADTrust/cdm-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickchandra/Documents/code/CADTrust/cdm-data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC7EA34-AF73-F046-8D7A-276E48D6CFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56877903-50EB-2A46-95A6-F046F3FA25B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="740" windowWidth="23340" windowHeight="17280" xr2:uid="{69D80E33-0C8E-184B-992C-0FA45A510B1F}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="29380" windowHeight="17280" xr2:uid="{69D80E33-0C8E-184B-992C-0FA45A510B1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1002">
   <si>
     <t>AD</t>
   </si>
@@ -3039,6 +3039,9 @@
   </si>
   <si>
     <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
   </si>
 </sst>
 </file>
@@ -3407,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0F8624-60DE-EC44-946A-37001F713615}">
   <dimension ref="A1:E246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4280,7 +4283,7 @@
         <v>93</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>93</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>